<commit_message>
Corrected excel import template
</commit_message>
<xml_diff>
--- a/public/templates/excel_import_template.xlsx
+++ b/public/templates/excel_import_template.xlsx
@@ -134,13 +134,13 @@
   <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="5" min="1" style="0" width="20.2040816326531"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="12.9591836734694"/>
+    <col collapsed="false" hidden="false" max="5" min="1" style="0" width="23.9948979591837"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="15.3877551020408"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>